<commit_message>
add radius difference analysis
</commit_message>
<xml_diff>
--- a/linreg_analysis/linreg.xlsx
+++ b/linreg_analysis/linreg.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F07291C-3A7D-45E0-8F5F-5056F7E3954D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06BD0C1-E16C-417B-9786-DF3CAFBD5092}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="2595" windowWidth="24360" windowHeight="13005" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$J$55</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Graphics!$A$1:$A$54</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Graphics!$B$1:$B$18</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Graphics!$C$1:$C$18</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Graphics!$B$1:$B$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Graphics!$C$1:$C$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Graphics!$A$1:$A$54</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Graphics!$D$1:$D$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -370,7 +370,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -432,7 +432,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -494,7 +494,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4893,7 +4893,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>